<commit_message>
modified DC converter calc
</commit_message>
<xml_diff>
--- a/latex/calc/DC_Converter_Calc.xlsx
+++ b/latex/calc/DC_Converter_Calc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Privat\Git\Projektarbeit-Hochvolt-Elektrik-Komponenten-FSE-Fahrzeug\latex\calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1604778-EE36-4885-B8AC-0D54F2F624FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121AB83E-CB32-4D16-B942-B3D7EF087127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -620,7 +620,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.000%"/>
-    <numFmt numFmtId="173" formatCode="0.00000"/>
+    <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -716,7 +716,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -748,10 +748,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -760,16 +766,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1881,8 +1880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E153" sqref="E153"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1895,17 +1894,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="36" t="s">
         <v>168</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -1939,7 +1938,7 @@
       <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="28" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2042,17 +2041,17 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -2102,14 +2101,14 @@
       <c r="A21" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="33">
+      <c r="B21" s="29">
         <f>(B5/B3)*B16</f>
         <v>5.75</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="33">
+      <c r="D21" s="29">
         <f>(B5/B3)*D16</f>
         <v>6.708333333333333</v>
       </c>
@@ -2250,17 +2249,17 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="36"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -2280,7 +2279,7 @@
       <c r="A33" t="s">
         <v>173</v>
       </c>
-      <c r="B33" s="34">
+      <c r="B33" s="30">
         <f>B32/B7</f>
         <v>0.1</v>
       </c>
@@ -2318,7 +2317,7 @@
       <c r="C35" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="33">
+      <c r="D35" s="29">
         <f>B35*10^6</f>
         <v>47.441130298273158</v>
       </c>
@@ -2343,7 +2342,7 @@
         <v>21</v>
       </c>
       <c r="B36" s="12">
-        <v>22.4</v>
+        <v>11.2</v>
       </c>
       <c r="C36" t="s">
         <v>13</v>
@@ -2366,9 +2365,9 @@
       <c r="A37" t="s">
         <v>188</v>
       </c>
-      <c r="B37" s="32">
+      <c r="B37" s="28">
         <f>B3/(B36*10^-6*B9)*(1-(B3/B6)*B23)</f>
-        <v>8.4716304104059219</v>
+        <v>16.943260820811844</v>
       </c>
       <c r="C37" t="s">
         <v>20</v>
@@ -2429,14 +2428,14 @@
       </c>
       <c r="B42" s="8">
         <f>B37/(8*B9*(D40-B32*B41))</f>
-        <v>4.5333630246423112E-5</v>
+        <v>9.0667260492846224E-5</v>
       </c>
       <c r="C42" t="s">
         <v>48</v>
       </c>
-      <c r="D42" s="33">
+      <c r="D42" s="29">
         <f>B42*10^6</f>
-        <v>45.333630246423112</v>
+        <v>90.667260492846225</v>
       </c>
       <c r="E42" t="s">
         <v>57</v>
@@ -2453,7 +2452,7 @@
       <c r="C44" t="s">
         <v>37</v>
       </c>
-      <c r="D44" s="33">
+      <c r="D44" s="29">
         <f>B44*10^3</f>
         <v>5.0718512256973787</v>
       </c>
@@ -2483,7 +2482,7 @@
       <c r="A47" t="s">
         <v>42</v>
       </c>
-      <c r="B47" s="35">
+      <c r="B47" s="31">
         <f>(D46*((1/((B5/1.25)-1))+1))/(B6/1.25)</f>
         <v>1994.9692080839623</v>
       </c>
@@ -2495,7 +2494,7 @@
       <c r="A48" t="s">
         <v>43</v>
       </c>
-      <c r="B48" s="35">
+      <c r="B48" s="31">
         <f>B47*((B6/1.25)-1)-D46</f>
         <v>3469.5116662330693</v>
       </c>
@@ -2547,14 +2546,14 @@
       <c r="A50" t="s">
         <v>39</v>
       </c>
-      <c r="B50" s="36">
+      <c r="B50" s="32">
         <f>(D16/(0.725*((B9/1000)/300)*(1.25/B49)))*51.1*10^3</f>
         <v>148013.79310345076</v>
       </c>
       <c r="C50" t="s">
         <v>46</v>
       </c>
-      <c r="D50" s="35">
+      <c r="D50" s="31">
         <f>B50*10^-3</f>
         <v>148.01379310345078</v>
       </c>
@@ -2582,17 +2581,17 @@
       </c>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A51" s="27" t="s">
+      <c r="A51" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="B51" s="27"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="27"/>
-      <c r="E51" s="27"/>
-      <c r="F51" s="27"/>
-      <c r="G51" s="27"/>
-      <c r="H51" s="27"/>
-      <c r="I51" s="27"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="36"/>
+      <c r="D51" s="36"/>
+      <c r="E51" s="36"/>
+      <c r="F51" s="36"/>
+      <c r="G51" s="36"/>
+      <c r="H51" s="36"/>
+      <c r="I51" s="36"/>
       <c r="R51" t="s">
         <v>84</v>
       </c>
@@ -2638,7 +2637,7 @@
       <c r="C53" t="s">
         <v>48</v>
       </c>
-      <c r="D53" s="37">
+      <c r="D53" s="33">
         <f>B53*10^9</f>
         <v>4.0605345564331667</v>
       </c>
@@ -2668,7 +2667,7 @@
       <c r="C54" t="s">
         <v>48</v>
       </c>
-      <c r="D54" s="37">
+      <c r="D54" s="33">
         <f>B54*10^9</f>
         <v>24.363207338599</v>
       </c>
@@ -2689,7 +2688,7 @@
       <c r="A56" t="s">
         <v>51</v>
       </c>
-      <c r="B56" s="35">
+      <c r="B56" s="31">
         <f>(1/(1-B18))*SQRT(B25*10^-6/B53)</f>
         <v>2296.9866312323384</v>
       </c>
@@ -2701,7 +2700,7 @@
       <c r="A58" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="32">
+      <c r="B58" s="28">
         <f>(1.2/(B9/B10))*22.1*10^6</f>
         <v>530.40000000000009</v>
       </c>
@@ -2710,17 +2709,17 @@
       </c>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A59" s="27" t="s">
+      <c r="A59" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="B59" s="27"/>
-      <c r="C59" s="27"/>
-      <c r="D59" s="27"/>
-      <c r="E59" s="27"/>
-      <c r="F59" s="27"/>
-      <c r="G59" s="27"/>
-      <c r="H59" s="27"/>
-      <c r="I59" s="27"/>
+      <c r="B59" s="36"/>
+      <c r="C59" s="36"/>
+      <c r="D59" s="36"/>
+      <c r="E59" s="36"/>
+      <c r="F59" s="36"/>
+      <c r="G59" s="36"/>
+      <c r="H59" s="36"/>
+      <c r="I59" s="36"/>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
@@ -2733,10 +2732,10 @@
       <c r="C60" t="s">
         <v>20</v>
       </c>
-      <c r="F60" s="30" t="s">
+      <c r="F60" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="G60" s="30"/>
+      <c r="G60" s="38"/>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
@@ -2749,8 +2748,8 @@
       <c r="D61" t="s">
         <v>104</v>
       </c>
-      <c r="F61" s="30"/>
-      <c r="G61" s="30"/>
+      <c r="F61" s="38"/>
+      <c r="G61" s="38"/>
       <c r="H61" t="s">
         <v>160</v>
       </c>
@@ -2761,13 +2760,13 @@
       </c>
       <c r="B62" s="18">
         <f>(1/B23)*(B7+(B37/2))</f>
-        <v>8.050918367346938</v>
+        <v>8.8218367346938784</v>
       </c>
       <c r="C62" t="s">
         <v>20</v>
       </c>
-      <c r="F62" s="30"/>
-      <c r="G62" s="30"/>
+      <c r="F62" s="38"/>
+      <c r="G62" s="38"/>
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B63" s="18"/>
@@ -2857,10 +2856,10 @@
     <row r="70" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B70" s="17"/>
       <c r="D70" s="4"/>
-      <c r="E70" s="28" t="s">
+      <c r="E70" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="F70" s="28"/>
+      <c r="F70" s="39"/>
       <c r="G70" s="23"/>
       <c r="R70" t="s">
         <v>83</v>
@@ -3016,17 +3015,17 @@
       <c r="G76" s="23"/>
     </row>
     <row r="77" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A77" s="27" t="s">
+      <c r="A77" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="B77" s="27"/>
-      <c r="C77" s="27"/>
-      <c r="D77" s="27"/>
-      <c r="E77" s="27"/>
-      <c r="F77" s="27"/>
-      <c r="G77" s="27"/>
-      <c r="H77" s="27"/>
-      <c r="I77" s="27"/>
+      <c r="B77" s="36"/>
+      <c r="C77" s="36"/>
+      <c r="D77" s="36"/>
+      <c r="E77" s="36"/>
+      <c r="F77" s="36"/>
+      <c r="G77" s="36"/>
+      <c r="H77" s="36"/>
+      <c r="I77" s="36"/>
     </row>
     <row r="78" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
@@ -3063,10 +3062,10 @@
       <c r="C80" t="s">
         <v>37</v>
       </c>
-      <c r="F80" s="30" t="s">
+      <c r="F80" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="G80" s="30"/>
+      <c r="G80" s="38"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
@@ -3085,8 +3084,8 @@
       <c r="E81" t="s">
         <v>111</v>
       </c>
-      <c r="F81" s="30"/>
-      <c r="G81" s="30"/>
+      <c r="F81" s="38"/>
+      <c r="G81" s="38"/>
       <c r="H81" t="s">
         <v>157</v>
       </c>
@@ -3108,8 +3107,8 @@
       <c r="E82" t="s">
         <v>111</v>
       </c>
-      <c r="F82" s="30"/>
-      <c r="G82" s="30"/>
+      <c r="F82" s="38"/>
+      <c r="G82" s="38"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
@@ -3315,17 +3314,17 @@
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A102" s="27" t="s">
+      <c r="A102" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="B102" s="27"/>
-      <c r="C102" s="27"/>
-      <c r="D102" s="27"/>
-      <c r="E102" s="27"/>
-      <c r="F102" s="27"/>
-      <c r="G102" s="27"/>
-      <c r="H102" s="27"/>
-      <c r="I102" s="27"/>
+      <c r="B102" s="36"/>
+      <c r="C102" s="36"/>
+      <c r="D102" s="36"/>
+      <c r="E102" s="36"/>
+      <c r="F102" s="36"/>
+      <c r="G102" s="36"/>
+      <c r="H102" s="36"/>
+      <c r="I102" s="36"/>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
@@ -3346,7 +3345,7 @@
       <c r="A104" t="s">
         <v>62</v>
       </c>
-      <c r="B104" s="38">
+      <c r="B104" s="34">
         <v>4.5</v>
       </c>
       <c r="C104" t="s">
@@ -3355,9 +3354,6 @@
       <c r="D104" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B105" s="39"/>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
@@ -3416,11 +3412,11 @@
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G109" s="29" t="s">
+      <c r="G109" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="H109" s="30"/>
-      <c r="I109" s="30"/>
+      <c r="H109" s="38"/>
+      <c r="I109" s="38"/>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
@@ -3435,9 +3431,9 @@
       <c r="D110" t="s">
         <v>171</v>
       </c>
-      <c r="G110" s="30"/>
-      <c r="H110" s="30"/>
-      <c r="I110" s="30"/>
+      <c r="G110" s="38"/>
+      <c r="H110" s="38"/>
+      <c r="I110" s="38"/>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
@@ -3449,9 +3445,9 @@
       <c r="C111" t="s">
         <v>9</v>
       </c>
-      <c r="G111" s="30"/>
-      <c r="H111" s="30"/>
-      <c r="I111" s="30"/>
+      <c r="G111" s="38"/>
+      <c r="H111" s="38"/>
+      <c r="I111" s="38"/>
       <c r="J111" t="s">
         <v>159</v>
       </c>
@@ -3460,37 +3456,37 @@
       <c r="A112" t="s">
         <v>65</v>
       </c>
-      <c r="B112" s="33">
+      <c r="B112" s="29">
         <f>B106*SQRT(2*B110*10^-3*((1.3*B111-B3)/(1.3*B111*B36*10^-6)))</f>
-        <v>3.2749465225060894</v>
+        <v>4.6314737881747163</v>
       </c>
       <c r="C112" t="s">
         <v>9</v>
       </c>
-      <c r="D112" s="40">
+      <c r="D112" s="35">
         <f>B112*10^3</f>
-        <v>3274.9465225060894</v>
+        <v>4631.473788174716</v>
       </c>
       <c r="E112" t="s">
         <v>64</v>
       </c>
-      <c r="G112" s="30"/>
-      <c r="H112" s="30"/>
-      <c r="I112" s="30"/>
+      <c r="G112" s="38"/>
+      <c r="H112" s="38"/>
+      <c r="I112" s="38"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>78</v>
       </c>
-      <c r="B113" s="33">
+      <c r="B113" s="29">
         <f>B112/B106</f>
-        <v>409.36831531326118</v>
+        <v>578.9342235218395</v>
       </c>
       <c r="C113" t="s">
         <v>20</v>
       </c>
       <c r="D113" s="12">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="E113" t="s">
         <v>20</v>
@@ -3522,16 +3518,16 @@
       <c r="A116" t="s">
         <v>73</v>
       </c>
-      <c r="B116" s="31">
+      <c r="B116" s="27">
         <f>((B115*40*10^-6)+66*10^-3)/D113</f>
-        <v>1.7666666666666668E-3</v>
+        <v>8.8333333333333341E-4</v>
       </c>
       <c r="C116" t="s">
         <v>37</v>
       </c>
-      <c r="D116" s="33">
+      <c r="D116" s="29">
         <f>B116*10^3</f>
-        <v>1.7666666666666668</v>
+        <v>0.88333333333333341</v>
       </c>
       <c r="E116" t="s">
         <v>38</v>
@@ -3553,9 +3549,9 @@
       <c r="A118" t="s">
         <v>125</v>
       </c>
-      <c r="B118" s="33">
+      <c r="B118" s="29">
         <f>SQRT((1-B17)*(B7^2+(B37^2/12)))</f>
-        <v>35.634613352465081</v>
+        <v>35.833116683549576</v>
       </c>
       <c r="C118" t="s">
         <v>20</v>
@@ -3586,7 +3582,7 @@
       </c>
       <c r="B120" s="17">
         <f>(B118^2*B106)+(B11*B9*B119)</f>
-        <v>10.503605350237462</v>
+        <v>10.617098010055033</v>
       </c>
       <c r="C120" t="s">
         <v>18</v>
@@ -3596,10 +3592,10 @@
     <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B121" s="17"/>
       <c r="D121" s="4"/>
-      <c r="E121" s="28" t="s">
+      <c r="E121" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="F121" s="28"/>
+      <c r="F121" s="39"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
@@ -3607,7 +3603,7 @@
       </c>
       <c r="B122" s="17">
         <f>(B14-B13)/B120</f>
-        <v>7.1404053655066564</v>
+        <v>7.0640772016016502</v>
       </c>
       <c r="C122" t="s">
         <v>146</v>
@@ -3690,7 +3686,7 @@
       </c>
       <c r="B127" s="17">
         <f>B122-B123-B124-B126</f>
-        <v>6.8847620724194085</v>
+        <v>6.8084339085144023</v>
       </c>
       <c r="C127" t="s">
         <v>146</v>
@@ -3730,26 +3726,26 @@
       <c r="A132" t="s">
         <v>166</v>
       </c>
-      <c r="B132" s="32">
+      <c r="B132" s="28">
         <f>B13+B120*B130</f>
-        <v>102.05212140713962</v>
+        <v>102.61455054557919</v>
       </c>
       <c r="C132" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A133" s="27" t="s">
+      <c r="A133" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="B133" s="27"/>
-      <c r="C133" s="27"/>
-      <c r="D133" s="27"/>
-      <c r="E133" s="27"/>
-      <c r="F133" s="27"/>
-      <c r="G133" s="27"/>
-      <c r="H133" s="27"/>
-      <c r="I133" s="27"/>
+      <c r="B133" s="36"/>
+      <c r="C133" s="36"/>
+      <c r="D133" s="36"/>
+      <c r="E133" s="36"/>
+      <c r="F133" s="36"/>
+      <c r="G133" s="36"/>
+      <c r="H133" s="36"/>
+      <c r="I133" s="36"/>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
@@ -3787,17 +3783,17 @@
       </c>
       <c r="B136">
         <f>SQRT(B18*(B7^2+(B37^2/12)))</f>
-        <v>30.344233465774721</v>
+        <v>30.513266629193211</v>
       </c>
       <c r="C136" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F137" s="30" t="s">
+      <c r="F137" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="G137" s="30"/>
+      <c r="G137" s="38"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
@@ -3817,8 +3813,8 @@
       <c r="E138" t="s">
         <v>38</v>
       </c>
-      <c r="F138" s="30"/>
-      <c r="G138" s="30"/>
+      <c r="F138" s="38"/>
+      <c r="G138" s="38"/>
       <c r="H138" t="s">
         <v>160</v>
       </c>
@@ -3840,8 +3836,8 @@
       <c r="E139" t="s">
         <v>111</v>
       </c>
-      <c r="F139" s="30"/>
-      <c r="G139" s="30"/>
+      <c r="F139" s="38"/>
+      <c r="G139" s="38"/>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
@@ -3849,7 +3845,7 @@
       </c>
       <c r="B141" s="24">
         <f>(B136^2*B138)+(B11*B139*B9)</f>
-        <v>2.0023759094359028</v>
+        <v>2.0233612583838418</v>
       </c>
       <c r="C141" t="s">
         <v>18</v>
@@ -3861,10 +3857,10 @@
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B143" s="17"/>
       <c r="D143" s="4"/>
-      <c r="E143" s="28" t="s">
+      <c r="E143" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="F143" s="28"/>
+      <c r="F143" s="39"/>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
@@ -3872,7 +3868,7 @@
       </c>
       <c r="B144" s="17">
         <f>(B14-B13)/B141</f>
-        <v>37.455504556648677</v>
+        <v>37.067033723827542</v>
       </c>
       <c r="C144" t="s">
         <v>146</v>
@@ -3947,7 +3943,7 @@
       </c>
       <c r="B149" s="17">
         <f>B144-B145-B146-B148</f>
-        <v>36.838556869075909</v>
+        <v>36.450086036254774</v>
       </c>
       <c r="C149" t="s">
         <v>146</v>
@@ -3992,24 +3988,24 @@
       </c>
       <c r="B154">
         <f>B13+B141*B152</f>
-        <v>75.263872100208729</v>
+        <v>75.528643150090346</v>
       </c>
       <c r="C154" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A155" s="27" t="s">
+      <c r="A155" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="B155" s="27"/>
-      <c r="C155" s="27"/>
-      <c r="D155" s="27"/>
-      <c r="E155" s="27"/>
-      <c r="F155" s="27"/>
-      <c r="G155" s="27"/>
-      <c r="H155" s="27"/>
-      <c r="I155" s="27"/>
+      <c r="B155" s="36"/>
+      <c r="C155" s="36"/>
+      <c r="D155" s="36"/>
+      <c r="E155" s="36"/>
+      <c r="F155" s="36"/>
+      <c r="G155" s="36"/>
+      <c r="H155" s="36"/>
+      <c r="I155" s="36"/>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
@@ -4062,6 +4058,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A155:I155"/>
+    <mergeCell ref="A51:I51"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="A102:I102"/>
+    <mergeCell ref="E121:F121"/>
+    <mergeCell ref="E143:F143"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="G109:I112"/>
     <mergeCell ref="A133:I133"/>
@@ -4071,13 +4074,6 @@
     <mergeCell ref="F80:G82"/>
     <mergeCell ref="F60:G62"/>
     <mergeCell ref="E70:F70"/>
-    <mergeCell ref="A155:I155"/>
-    <mergeCell ref="A51:I51"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="A31:I31"/>
-    <mergeCell ref="A102:I102"/>
-    <mergeCell ref="E121:F121"/>
-    <mergeCell ref="E143:F143"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>